<commit_message>
homepage billboard sections added
</commit_message>
<xml_diff>
--- a/cadence-template.xlsx
+++ b/cadence-template.xlsx
@@ -2,22 +2,25 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arthur.lurye/Documents/cadence-generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{321608AF-937F-084E-956D-C82FADE19195}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E75662D-940F-B943-981A-F376FB9174AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5200" yWindow="1480" windowWidth="29240" windowHeight="16940" xr2:uid="{49AB680B-4460-7D4B-AC28-ED89FA0896F3}"/>
+    <workbookView xWindow="4020" yWindow="2380" windowWidth="29240" windowHeight="16940" activeTab="5" xr2:uid="{49AB680B-4460-7D4B-AC28-ED89FA0896F3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Promo Short Billboard" sheetId="2" r:id="rId1"/>
-    <sheet name="Html Ads" sheetId="6" r:id="rId2"/>
-    <sheet name="heroBanners" sheetId="1" r:id="rId3"/>
+    <sheet name="Homepage Billboards" sheetId="15" r:id="rId1"/>
+    <sheet name="Promo Short Billboard" sheetId="2" r:id="rId2"/>
+    <sheet name="Html Ads" sheetId="6" r:id="rId3"/>
     <sheet name="Feature Product Spotlight" sheetId="3" r:id="rId4"/>
-    <sheet name="Cross Promos" sheetId="5" r:id="rId5"/>
+    <sheet name="Health Fitness Section" sheetId="16" r:id="rId5"/>
+    <sheet name="Cross Promos" sheetId="10" r:id="rId6"/>
+    <sheet name="Deals Drawer Main" sheetId="12" r:id="rId7"/>
+    <sheet name="heroBanners" sheetId="13" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="247">
   <si>
     <t>name</t>
   </si>
@@ -121,78 +124,12 @@
     <t>postHeaderText3</t>
   </si>
   <si>
-    <t>icon</t>
-  </si>
-  <si>
-    <t>BOGO50VSB_012720_Web_L3</t>
-  </si>
-  <si>
-    <t>Nourish yourself, inside and out. with naturally-sourced products from top beauty brands including Reserveage!</t>
-  </si>
-  <si>
-    <t>SHOP SALE &gt;</t>
-  </si>
-  <si>
-    <t>SHOP NOW &gt;</t>
-  </si>
-  <si>
     <t>/b/women-s-best/N-cp9a6g</t>
   </si>
   <si>
-    <t>WEB WK8 021720 Digestive Event 105625_Web_SecondaryBillboard</t>
-  </si>
-  <si>
-    <t>ng-click="asset.promoClick({id :  '2002_4 Day Digestive event 20p off Promotional Short Billboard 1', position : 'Promotional Short Billboard 1', name : '2002_4 Day Digestive event 20p off', creative: '20% Off'})"</t>
-  </si>
-  <si>
-    <t>/c/digestive-health-sale/N-cp99y8</t>
-  </si>
-  <si>
-    <t>Limited Time Only: Up To 20% Off Digestive Support</t>
-  </si>
-  <si>
-    <t>Nourish your gut with the right mix of probiotic strains featuring active bacterial cultures.</t>
-  </si>
-  <si>
-    <t>WomensBestLaunch_BOGO50_020320_SecondaryBillboard_01</t>
-  </si>
-  <si>
-    <t>ng-click="asset.promoClick({id :  '2002_Womens Best Launch and BOGO50 Promotional Short Billboard 2', position : 'Promotional Short Billboard 2', name : '2002_Womens Best Launch and BOGO50', creative: 'BOGO50'})"</t>
-  </si>
-  <si>
-    <t>BOGO 50% Off NEW Women's Best&lt;sup&gt;&amp;trade;&lt;/sup&gt; Premium Supplements</t>
-  </si>
-  <si>
-    <t>ng-click="asset.promoClick({id :  '2002_Solaray Leaf therapeutics cbd 20p off Promotional Short Billboard 3', position : 'Promotional Short Billboard 3', name : '2002_Solaray Leaf therapeutics cbd 20p off', creative: '20% Off'})"</t>
-  </si>
-  <si>
-    <t>/c/cbd-hemp-extract/solaray/N-cp9a1pZ9b0</t>
-  </si>
-  <si>
-    <t>SOLARAY_20OFF_012720_Web_SecondaryBillboard</t>
-  </si>
-  <si>
-    <t>20% Off Leaf Therapeutics Hemp Extract By Solaray</t>
-  </si>
-  <si>
-    <t>Explore hemp extract for balance—plus targeted blends for pain &amp; sleep—with a full spectrum array of beneficial phytocannabinoids.</t>
-  </si>
-  <si>
-    <t>ng-click="asset.promoClick({id :  '2002_Jocko Lauch Promotional Short Billboard 4', position : 'Promotional Short Billboard 4', name : '2002_Jocko Lauch', creative: 'General'})"</t>
-  </si>
-  <si>
     <t>/b/jocko-fuel/N-cp9a4i</t>
   </si>
   <si>
-    <t>Jocko_newbrandlaunch_012720_Web_SecondaryBillboard</t>
-  </si>
-  <si>
-    <t>Introducing Jocko Fuel</t>
-  </si>
-  <si>
-    <t>Built to work. Made for life. These new supplements are backed by science &amp; developed with retired Navy Seal Jocko Willink.</t>
-  </si>
-  <si>
     <t>width</t>
   </si>
   <si>
@@ -307,9 +244,6 @@
     <t>/p/burner-120-capsules/wbe0026</t>
   </si>
   <si>
-    <t>EASYSHOP</t>
-  </si>
-  <si>
     <t>2-AQ-WK-9-EASYPICKUP_VA_160x600_1_02</t>
   </si>
   <si>
@@ -328,71 +262,530 @@
     <t>with 2-Hour Pickup</t>
   </si>
   <si>
-    <t>S_2002_Cold and Flu</t>
-  </si>
-  <si>
-    <t>ng-click="asset.promoClick({id : '2002_Cold and Flu Hero Banner', position : 'Hero Banner', name : '2002_Cold and Flu', creative: 'General'})"</t>
-  </si>
-  <si>
-    <t>/c/cold-flu/N-cp99mb</t>
-  </si>
-  <si>
-    <t>Try our favorite Homeopathic remedies</t>
-  </si>
-  <si>
-    <t>Survive Flu Season</t>
-  </si>
-  <si>
-    <t>GET-EM QUICK!</t>
-  </si>
-  <si>
-    <t>2002_Cold and Flu</t>
-  </si>
-  <si>
-    <t>2002_Cold and Flu V2</t>
-  </si>
-  <si>
-    <t>3 HOMEOPATHIC MEDICINES TO HELP YOU SURVIVE COLD &amp; FLU SEASON</t>
-  </si>
-  <si>
-    <t>Oscillococcinum, Chestal Honey, &amp; Coldcalm use natural extracts to help you bounce back. Here’s what to know about them.</t>
-  </si>
-  <si>
-    <t>CHECK IT OUT</t>
-  </si>
-  <si>
-    <t>#CEDFD7</t>
-  </si>
-  <si>
-    <t>cold</t>
-  </si>
-  <si>
-    <t>#EED7DF</t>
-  </si>
-  <si>
-    <t>flu</t>
-  </si>
-  <si>
-    <t>COLD-&amp;-FLU-Supporting-assets-115185_CPCMcontent</t>
-  </si>
-  <si>
-    <t>COLD-&amp;-FLU-Supporting-assets-115185_CPCMprod</t>
-  </si>
-  <si>
-    <t>SURVIVE FLU SEASON WITH OUR FAVE HOMEOPATHIC REMEDIES</t>
-  </si>
-  <si>
-    <t>Flu got you down? Get back up with 2-Hour Pickup for Oscilliococcinum, Chestal Honey, Cold Calm, Flu Fix, and more.</t>
-  </si>
-  <si>
-    <t>GET'EM QUICK!</t>
+    <t>badge1</t>
+  </si>
+  <si>
+    <t>badge2</t>
+  </si>
+  <si>
+    <t>/b/vital-proteins/N-cp99bc</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>20% OFF</t>
+  </si>
+  <si>
+    <t>/b/plnt/N-cp983o</t>
+  </si>
+  <si>
+    <t>/b/new-chapter/N-985</t>
+  </si>
+  <si>
+    <t>SHOP NOW</t>
+  </si>
+  <si>
+    <t>PLAYER20</t>
+  </si>
+  <si>
+    <t>postHeaderText1</t>
+  </si>
+  <si>
+    <t>mobileImageName</t>
+  </si>
+  <si>
+    <t>desktopImageName</t>
+  </si>
+  <si>
+    <t>2003_CHAMPION 20p off 2 items</t>
+  </si>
+  <si>
+    <t>ng-click="asset.promoClick({id :  '2003_CHAMPION 20p off 2 items Deals Drawer Left Main Feature', position : 'Deals Drawer Left Main Feature', name : '2003_CHAMPION 20p off 2 items', creative: '20% Off'})"</t>
+  </si>
+  <si>
+    <t>CHAMPIONCoupon_MobileBillboard</t>
+  </si>
+  <si>
+    <t>CHAMPIONCoupon_HPBillboard</t>
+  </si>
+  <si>
+    <t>any 2 items (or more) &lt;sup&gt;*&lt;/sup&gt;</t>
+  </si>
+  <si>
+    <t>CHAMPIONCoupon_D1</t>
+  </si>
+  <si>
+    <t>any 2 items (or more)&lt;sup&gt;*&lt;/sup&gt;</t>
+  </si>
+  <si>
+    <t>Online | Use code: &lt;span&gt;CHAMPION&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>2003_MVP Sale Up to 20p off</t>
+  </si>
+  <si>
+    <t>/c/mvp-brands-sale/N-cp9a8e</t>
+  </si>
+  <si>
+    <t>ng-click="asset.promoClick({id :  '2003_MVP Sale Up to 20p off Deals Drawer Left Main Feature', position : 'Deals Drawer Left Main Feature', name : '2003_MVP Sale Up to 20p off', creative: 'Up to 20% Off'})"</t>
+  </si>
+  <si>
+    <t>MVPSALE_upto20off_0224_D1</t>
+  </si>
+  <si>
+    <t>UP TO</t>
+  </si>
+  <si>
+    <t>Save on your favorite vitamins, collagen, digestive support, and more!</t>
+  </si>
+  <si>
+    <t>Shop Sale</t>
+  </si>
+  <si>
+    <t>subtitle</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>pretitle</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>AGuideToGraduallyGettingBackIntoYourGymGroove_RESPONSIVE_C</t>
+  </si>
+  <si>
+    <t>data-promoclick="{id :  '2006_Whats Good Testosterone PLP Homepage Content Module 2', position : 'Homepage Content Module 2', name : '2006_Whats Good Testosterone PLP', creative: 'General'}"</t>
+  </si>
+  <si>
+    <t>/c/testosterone-boosters/N-cp99ji</t>
+  </si>
+  <si>
+    <t>What's Good: Testosterone Boosters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Level up and get back in the game with our best testosterone-supporting supps from brands you can trust. </t>
+  </si>
+  <si>
+    <t>Save 20% on &lt;br&gt; Bucked Up</t>
+  </si>
+  <si>
+    <t>BOGO 50% Off Heart &lt;br&gt; Health &amp;amp; Omega Faves</t>
+  </si>
+  <si>
+    <t>CELSIUS_BOGO50_SUMMERSIPS_RESPONSIVE_B</t>
+  </si>
+  <si>
+    <t>BOGO 50% Off &lt;br&gt; Celsius Fitness Drink Cases</t>
+  </si>
+  <si>
+    <t>VSB_BOGO50_062920_RESPONSIVE_B</t>
+  </si>
+  <si>
+    <t>WOMENSBEST_B2G1_062920_RESPONSIVE_B</t>
+  </si>
+  <si>
+    <t>S_2007_JULY1776 25p or 17p off</t>
+  </si>
+  <si>
+    <t>ng-click="asset.promoClick({id :  '2007_JULY1776 25p or 17p off Hero Banner', position : 'Hero Banner', name : '2007_JULY1776 25p or 17p off', creative: 'Buy More Save More'})"</t>
+  </si>
+  <si>
+    <t>JULY1776_Coupon_L3</t>
+  </si>
+  <si>
+    <t>25% OFF $150</t>
+  </si>
+  <si>
+    <t>17% OFF $76*</t>
+  </si>
+  <si>
+    <t>PLUS FREE SHIPPING</t>
+  </si>
+  <si>
+    <t>Online Only | Use Code: &lt;strong&gt;JULY1776&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t>S_2007_New Chapter BOGO50</t>
+  </si>
+  <si>
+    <t>ng-click="asset.promoClick({id :  '2007_New Chapter BOGO50 Hero Banner', position : 'Hero Banner', name : '2007_New Chapter BOGO50', creative: 'BOGO50'})"</t>
+  </si>
+  <si>
+    <t>NEWCHAPTER_BOGO50_062920_L3</t>
+  </si>
+  <si>
+    <t>50% OFF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Chapter </t>
+  </si>
+  <si>
+    <t>S_2007_NeoCell BOGO50</t>
+  </si>
+  <si>
+    <t>ng-click="asset.promoClick({id :  '2007_NeoCell BOGO50 Hero Banner', position : 'Hero Banner', name : '2007_NeoCell BOGO50', creative: 'BOGO50'})"</t>
+  </si>
+  <si>
+    <t>/b/neocell/N-983</t>
+  </si>
+  <si>
+    <t>NEOCELL_BOGO50_062920_L3</t>
+  </si>
+  <si>
+    <t>NewCell</t>
+  </si>
+  <si>
+    <t>Activate your Inner beauty with collagen for healthy hair, skin, nails &amp;amp; more!</t>
+  </si>
+  <si>
+    <t>S_2007_True Athlete 20p off</t>
+  </si>
+  <si>
+    <t>ng-click="asset.promoClick({id :  '2007_True Athlete 20p off Hero Banner', position : 'Hero Banner', name : '2007_True Athlete 20p off', creative: '20% Off'})"</t>
+  </si>
+  <si>
+    <t>/b/true-athlete/N-9cc</t>
+  </si>
+  <si>
+    <t>TRUEATHLETE_20OFF_062920_L3</t>
+  </si>
+  <si>
+    <t>TrueAthlete&lt;sup&gt;&amp;reg;&lt;/sup&gt; sports nutrition</t>
+  </si>
+  <si>
+    <t>Get cleaner peformance support with NSF&lt;sup&gt;&amp;reg;&lt;/sup&gt;&lt;br&gt; Certified for Sport&lt;sup&gt;&amp;reg;&lt;/sup&gt;  pre-, intra-, and post-workout supplements.</t>
+  </si>
+  <si>
+    <t>S_2007_Outright Bars BOGO50</t>
+  </si>
+  <si>
+    <t>ng-click="asset.promoClick({id :  '2007_Outright Bars BOGO50 Hero Banner', position : 'Hero Banner', name : '2007_Outright Bars BOGO50', creative: 'BOGO50'})"</t>
+  </si>
+  <si>
+    <t>/b/mts-nutrition/N-cp9a6e</t>
+  </si>
+  <si>
+    <t>OUTRIGHTBARS_BOGO50_L3</t>
+  </si>
+  <si>
+    <t>Outright protein bar cases</t>
+  </si>
+  <si>
+    <t>S_2007_Jocko Fuel 20p off</t>
+  </si>
+  <si>
+    <t>ng-click="asset.promoClick({id :  '2007_Jocko Fuel 20p off Hero Banner', position : 'Hero Banner', name : '2007_Jocko Fuel 20p off', creative: '20% Off'})"</t>
+  </si>
+  <si>
+    <t>JOCKOFUEL_20OFF_062920_L3</t>
+  </si>
+  <si>
+    <t>S_2007_Xtend 2 for 50d</t>
+  </si>
+  <si>
+    <t>ng-click="asset.promoClick({id :  '2007_Xtend 2 for 50d Hero Banner', position : 'Hero Banner', name : '2007_Xtend 2 for 50d', creative: 'Buy X Get $X Off'})"</t>
+  </si>
+  <si>
+    <t>/b/xtend/N-cp9a7z</t>
+  </si>
+  <si>
+    <t>XTEND_2FOR50_L3</t>
+  </si>
+  <si>
+    <t>Get Your XTEND Favorites</t>
+  </si>
+  <si>
+    <t>2 for $50</t>
+  </si>
+  <si>
+    <t>S_2007_Vitamin Angels</t>
+  </si>
+  <si>
+    <t>ng-click="asset.promoClick({id :  '2007_Vitamin Angels Hero Banner', position : 'Hero Banner', name : '2007_Vitamin Angels', creative: 'General'})"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/p/vitamin-angels-bracelet-1-bracelet-s/xy-0289 </t>
+  </si>
+  <si>
+    <t>VITAMINANGELS_CAMPAIGN_L3</t>
+  </si>
+  <si>
+    <t>Help Every Child Shine</t>
+  </si>
+  <si>
+    <t>Purchase a handmade $5 bracelet crafted by communities in Guatemala and all proceeds will be donated to Vitamin Angels.</t>
+  </si>
+  <si>
+    <t>Learn More</t>
+  </si>
+  <si>
+    <t>S_2007_Raze BOGO50 Summer sips</t>
+  </si>
+  <si>
+    <t>ng-click="asset.promoClick({id :  '2007_Raze BOGO50 Summer sips Hero Banner', position : 'Hero Banner', name : '2007_Raze BOGO50 Summer sips', creative: 'BOGO50'})"</t>
+  </si>
+  <si>
+    <t>/b/repp-sports/N-cp9a6f</t>
+  </si>
+  <si>
+    <t>RAZE_BOGO50_SUMMERSIPS_L3</t>
+  </si>
+  <si>
+    <t>Raze energy drink cases</t>
+  </si>
+  <si>
+    <t>Fuel Up</t>
+  </si>
+  <si>
+    <t>/c/supplements/the-vitamin-shoppe/N-cp99iaZ9c1</t>
+  </si>
+  <si>
+    <t>data-promoclick="{id :  '2007_VSB Heart Health and Omegas BOGO50 Homepage Round Billboard 1', position : 'Homepage Round Billboard 1', name : '2007_VSB Heart Health and Omegas BOGO50', creative: 'BOGO50'}"</t>
+  </si>
+  <si>
+    <t>/b/celsius/N-91r</t>
+  </si>
+  <si>
+    <t>data-promoclick="{id :  '2007_Celsius BOGO50 Summer sips Homepage Round Billboard 2', position : 'Homepage Round Billboard 2', name : '2007_Celsius BOGO50 Summer sips', creative: 'BOGO50'}"</t>
+  </si>
+  <si>
+    <t>Buy Two, Get One FREE: &lt;br&gt; Women's Best</t>
+  </si>
+  <si>
+    <t>data-promoclick="{id :  '2007_Womens Best B2G1 Free Homepage Round Billboard 3', position : 'Homepage Round Billboard 3', name : '2007_Womens Best B2G1 Free', creative: 'Buy X Get X Free'}"</t>
+  </si>
+  <si>
+    <t>/b/bucked-up/N-cp99s0</t>
+  </si>
+  <si>
+    <t>data-promoclick="{id :  '2007_Bucked Up 20p off Homepage Round Billboard 4', position : 'Homepage Round Billboard 4', name : '2007_Bucked Up 20p off', creative: '20% Off'}"</t>
+  </si>
+  <si>
+    <t>BUCKEDUP_20OFF_062920_RESPONSIVE_B</t>
+  </si>
+  <si>
+    <t>Buy One, Get One</t>
+  </si>
+  <si>
+    <t>2007_plnt BOGO50</t>
+  </si>
+  <si>
+    <t>ng-click="asset.promoClick({id :  '2007_plnt BOGO50 Cross Promo Module', position : 'Cross Promo Module', name : '2007_plnt BOGO50', creative: 'BOGO50'})"</t>
+  </si>
+  <si>
+    <t>PLNT_BOGO50_062920_CPCM</t>
+  </si>
+  <si>
+    <t>#dfe0e2</t>
+  </si>
+  <si>
+    <t>BOGO 50% Off &lt;br&gt;The plnt&lt;sup&gt;&amp;reg;&lt;/sup&gt; Brand</t>
+  </si>
+  <si>
+    <t>Save on Earth-friendly protein, herbs &amp; more, independently tested for purity, potency &amp; quality.</t>
+  </si>
+  <si>
+    <t>plnt</t>
+  </si>
+  <si>
+    <t>2007_Whats Good Thermogenics</t>
+  </si>
+  <si>
+    <t>tbd</t>
+  </si>
+  <si>
+    <t>ng-click="asset.promoClick({id :  '2007_Whats Good Thermogenics Cross Promo Module', position : 'Cross Promo Module', name : '2007_Whats Good Thermogenics', creative: 'General'})"</t>
+  </si>
+  <si>
+    <t>Thermogenics_PLP_062920__CPCM</t>
+  </si>
+  <si>
+    <t>#c9ebf5</t>
+  </si>
+  <si>
+    <t>What's Good: Thermogenics</t>
+  </si>
+  <si>
+    <t>Heat up your training routine with fat- &amp; calorie-burning support to kick your goals into overdrive.</t>
+  </si>
+  <si>
+    <t>thermo</t>
+  </si>
+  <si>
+    <t>2007_Vitamin Angels</t>
+  </si>
+  <si>
+    <t>ng-click="asset.promoClick({id :  '2007_Vitamin Angels Cross Promo Module', position : 'Cross Promo Module', name : '2007_Vitamin Angels', creative: 'General'})"</t>
+  </si>
+  <si>
+    <t>VITAMINANGELS_CAMPAIGN_CPCM</t>
+  </si>
+  <si>
+    <t>#007889</t>
+  </si>
+  <si>
+    <t>Purchase a handmade $5 bracelet and all proceeds will be donated to Vitamin Angels.</t>
+  </si>
+  <si>
+    <t>va</t>
+  </si>
+  <si>
+    <t>2007_New Papa and Barkley</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>ng-click="asset.promoClick({id :  '2007_New Papa and Barkley Cross Promo Module', position : 'Cross Promo Module', name : '2007_New Papa and Barkley', creative: 'General'})"</t>
+  </si>
+  <si>
+    <t>PAPABARKLEY_NEWLAUNCH_CPCM</t>
+  </si>
+  <si>
+    <t>#fadbbe</t>
+  </si>
+  <si>
+    <t>Introducing Papa &amp; Barkley</t>
+  </si>
+  <si>
+    <t>Our newest CBD brand brings you 100% natural, clean, &amp; simple CBD Releaf in soothing balms, body oils, &amp; more.</t>
+  </si>
+  <si>
+    <t>Shop Papa &amp; Barkley</t>
+  </si>
+  <si>
+    <t>bark</t>
+  </si>
+  <si>
+    <t>2007_New Supps ft Rainbow light Natural factors MegaFood</t>
+  </si>
+  <si>
+    <t>/c/bogo50-rainbow-light-neocell-natural-vitality-renew-life/N-cp99y9</t>
+  </si>
+  <si>
+    <t>ng-click="asset.promoClick({id :  '2007_New Supps ft Rainbow light Natural factors MegaFood Cross Promo Module', position : 'Cross Promo Module', name : '2007_New Supps ft Rainbow light Natural factors MegaFood', creative: 'General'})"</t>
+  </si>
+  <si>
+    <t>NEWSUPPLEMENTS_RAINBOWLIGHT_ NATURAL FACTOR_MEGAFOOD_CPCM_</t>
+  </si>
+  <si>
+    <t>#fddccb</t>
+  </si>
+  <si>
+    <t>New In Women's Health</t>
+  </si>
+  <si>
+    <t>Try the latest from Rainbow Light, Natural Factors, &amp; more.</t>
+  </si>
+  <si>
+    <t>rainbow</t>
+  </si>
+  <si>
+    <t>2007_New Jym</t>
+  </si>
+  <si>
+    <t>ng-click="asset.promoClick({id :  '2007_New Jym Cross Promo Module', position : 'Cross Promo Module', name : '2007_New Jym', creative: 'General'})"</t>
+  </si>
+  <si>
+    <t>JYMlaunch_062920 _CPCM</t>
+  </si>
+  <si>
+    <t>#dce0e3</t>
+  </si>
+  <si>
+    <t>Just in: JYM!</t>
+  </si>
+  <si>
+    <t>Try PRO JYM Ultra-Premium Protein blend with top ingredients for strength &amp; size—exclusively online!</t>
+  </si>
+  <si>
+    <t>jym</t>
+  </si>
+  <si>
+    <t>2007_Womens Best B2G1 Free</t>
+  </si>
+  <si>
+    <t>ng-click="asset.promoClick({id :  '2007_Womens Best B2G1 Free Cross Promo Module', position : 'Cross Promo Module', name : '2007_Womens Best B2G1 Free', creative: 'Buy X Get X Free'})"</t>
+  </si>
+  <si>
+    <t>WOMENSBEST_B2G1_062920_CPCM</t>
+  </si>
+  <si>
+    <t>#f4f4f4</t>
+  </si>
+  <si>
+    <t>Buy Two, Get One FREE: Women’s Best</t>
+  </si>
+  <si>
+    <t>Get your HERcules on, with sports nutrition made for women.</t>
+  </si>
+  <si>
+    <t>womens</t>
+  </si>
+  <si>
+    <t>2007_Vital Proteins BOGO50</t>
+  </si>
+  <si>
+    <t>ng-click="asset.promoClick({id :  '2007_Vital Proteins BOGO50 Cross Promo Module', position : 'Cross Promo Module', name : '2007_Vital Proteins BOGO50', creative: 'BOGO50'})"</t>
+  </si>
+  <si>
+    <t>VITALPROTEINS_BOGO50_062920__CPCM_</t>
+  </si>
+  <si>
+    <t>#fae5ea</t>
+  </si>
+  <si>
+    <t>BOGO 50% Off Vital Proteins</t>
+  </si>
+  <si>
+    <t>Save on America’s #1 Collagen brand-no added sugars, fillers, binders, or artificial sweeteners.</t>
+  </si>
+  <si>
+    <t>vital</t>
+  </si>
+  <si>
+    <t>2007_True Athlete 20p off</t>
+  </si>
+  <si>
+    <t>ng-click="asset.promoClick({id :  '2007_True Athlete 20p off Cross Promo Module', position : 'Cross Promo Module', name : '2007_True Athlete 20p off', creative: '20% Off'})"</t>
+  </si>
+  <si>
+    <t>TRUEATHLETE_20OFF_062920_CPCM</t>
+  </si>
+  <si>
+    <t>#fadbaf</t>
+  </si>
+  <si>
+    <t>True Athlete&lt;sup&gt;&amp;reg;&lt;/sup&gt;= &lt;br&gt; Cleaner Performance</t>
+  </si>
+  <si>
+    <t>Explore the NEWEST NSF® Certified for Sport1 supps, like Endurance &amp; Recovery, Pure Pre, &amp; more.</t>
+  </si>
+  <si>
+    <t>tap</t>
+  </si>
+  <si>
+    <t>2007_True Athlete V2 (no promo)</t>
+  </si>
+  <si>
+    <t>ng-click="asset.promoClick({id :  '2007_True Athlete V2 Cross Promo Module', position : 'Cross Promo Module', name : '2007_True Athlete V2', creative: 'General'})"</t>
+  </si>
+  <si>
+    <t>20% Off True Athlete&lt;sup&gt;&amp;reg;&lt;/sup&gt;</t>
+  </si>
+  <si>
+    <t>tanp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -452,13 +845,66 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF172B4D"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0563C1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -489,7 +935,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -498,6 +944,19 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -812,11 +1271,126 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F71BD111-09A2-1A4D-88C0-F8C423BC7275}">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G4" t="s">
+        <v>90</v>
+      </c>
+      <c r="H4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1FEE12E-A1B2-7945-8CDA-9BE45F21A83A}">
-  <dimension ref="A1:F5"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -828,7 +1402,7 @@
     <col min="5" max="5" width="29.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -841,91 +1415,61 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" t="s">
-        <v>35</v>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>168</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>114</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" t="s">
-        <v>40</v>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>170</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>115</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" t="s">
-        <v>42</v>
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>172</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>112</v>
       </c>
       <c r="D4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" t="s">
-        <v>47</v>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>174</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>175</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F5" t="s">
-        <v>32</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -933,12 +1477,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4278EB63-4F71-694C-B5B9-FD13E4D359B2}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -954,10 +1499,10 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -969,22 +1514,22 @@
         <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>4</v>
@@ -998,22 +1543,22 @@
         <v>600</v>
       </c>
       <c r="C2" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="G2" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="J2" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="K2" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="L2" t="s">
         <v>8</v>
@@ -1027,22 +1572,22 @@
         <v>250</v>
       </c>
       <c r="C3" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D3" t="s">
         <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="G3" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="J3" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="K3" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="L3" t="s">
         <v>8</v>
@@ -1056,22 +1601,22 @@
         <v>600</v>
       </c>
       <c r="C4" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D4" t="s">
         <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
       <c r="G4" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="J4" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="K4" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="L4" t="s">
         <v>8</v>
@@ -1085,19 +1630,19 @@
         <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D5" t="s">
         <v>25</v>
       </c>
       <c r="G5" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="J5" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="K5" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="L5" t="s">
         <v>8</v>
@@ -1111,22 +1656,22 @@
         <v>90</v>
       </c>
       <c r="C6" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D6" t="s">
         <v>25</v>
       </c>
       <c r="E6" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="G6" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="J6" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="K6" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="L6" t="s">
         <v>8</v>
@@ -1140,108 +1685,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CCEFC6D-EE13-EF4B-A2EA-D63CE352C75D}">
-  <dimension ref="A1:K8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="20.33203125" customWidth="1"/>
-    <col min="7" max="8" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.1640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="H2" t="s">
-        <v>100</v>
-      </c>
-      <c r="K2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B8" s="4"/>
-      <c r="G8" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{051D40BC-4E57-B643-A271-0662EA5CA887}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1282,19 +1728,19 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="D2">
         <v>2196525</v>
       </c>
       <c r="E2" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="F2" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1302,19 +1748,19 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="D3">
         <v>2193076</v>
       </c>
       <c r="E3" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="F3" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1322,19 +1768,19 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="D4">
         <v>2200442</v>
       </c>
       <c r="E4" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="F4" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1342,10 +1788,10 @@
         <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="D5">
         <v>1655208</v>
@@ -1354,7 +1800,7 @@
         <v>24</v>
       </c>
       <c r="F5" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1362,10 +1808,10 @@
         <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="C6" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="D6">
         <v>2189884</v>
@@ -1374,7 +1820,7 @@
         <v>20</v>
       </c>
       <c r="F6" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1382,19 +1828,19 @@
         <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="C7" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="D7">
         <v>2190346</v>
       </c>
       <c r="E7" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="F7" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1402,19 +1848,19 @@
         <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C8" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="D8">
         <v>2188142</v>
       </c>
       <c r="E8" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="F8" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1422,10 +1868,10 @@
         <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="C9" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="D9">
         <v>2197226</v>
@@ -1434,7 +1880,7 @@
         <v>16</v>
       </c>
       <c r="F9" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1443,14 +1889,126 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCC0B53C-AAA7-924F-B6FF-DE89B05511AA}">
-  <dimension ref="A1:I3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E2BA05F-0B98-B74A-8B8D-9470A88557B2}">
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>109</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4011476-088C-6247-949E-CF09A321B5BF}">
+  <sheetPr codeName="Sheet7"/>
+  <dimension ref="A1:I11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="56.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.83203125" customWidth="1"/>
+    <col min="4" max="4" width="61.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
@@ -1481,62 +2039,692 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="D3" t="s">
+        <v>187</v>
+      </c>
+      <c r="E3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F3" t="s">
+        <v>189</v>
+      </c>
+      <c r="G3" t="s">
+        <v>190</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="D4" t="s">
+        <v>194</v>
+      </c>
+      <c r="E4" t="s">
+        <v>195</v>
+      </c>
+      <c r="F4" t="s">
+        <v>158</v>
+      </c>
+      <c r="G4" t="s">
+        <v>196</v>
+      </c>
+      <c r="H4" t="s">
+        <v>160</v>
+      </c>
+      <c r="I4" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="D5" t="s">
+        <v>201</v>
+      </c>
+      <c r="E5" t="s">
+        <v>202</v>
+      </c>
+      <c r="F5" t="s">
+        <v>203</v>
+      </c>
+      <c r="G5" t="s">
+        <v>204</v>
+      </c>
+      <c r="H5" t="s">
+        <v>205</v>
+      </c>
+      <c r="I5" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="D6" t="s">
+        <v>210</v>
+      </c>
+      <c r="E6" t="s">
+        <v>211</v>
+      </c>
+      <c r="F6" t="s">
+        <v>212</v>
+      </c>
+      <c r="G6" t="s">
+        <v>213</v>
+      </c>
+      <c r="H6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="D7" t="s">
+        <v>217</v>
+      </c>
+      <c r="E7" t="s">
+        <v>218</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="G7" t="s">
+        <v>220</v>
+      </c>
+      <c r="H7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>222</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="D8" t="s">
+        <v>224</v>
+      </c>
+      <c r="E8" t="s">
+        <v>225</v>
+      </c>
+      <c r="F8" t="s">
+        <v>226</v>
+      </c>
+      <c r="G8" t="s">
+        <v>227</v>
+      </c>
+      <c r="H8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>229</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="D9" t="s">
+        <v>231</v>
+      </c>
+      <c r="E9" t="s">
+        <v>232</v>
+      </c>
+      <c r="F9" t="s">
+        <v>233</v>
+      </c>
+      <c r="G9" t="s">
+        <v>234</v>
+      </c>
+      <c r="H9" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>236</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="D10" t="s">
+        <v>238</v>
+      </c>
+      <c r="E10" t="s">
+        <v>239</v>
+      </c>
+      <c r="F10" t="s">
+        <v>240</v>
+      </c>
+      <c r="G10" t="s">
+        <v>241</v>
+      </c>
+      <c r="H10" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>243</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="D11" t="s">
+        <v>238</v>
+      </c>
+      <c r="E11" t="s">
+        <v>239</v>
+      </c>
+      <c r="F11" t="s">
+        <v>245</v>
+      </c>
+      <c r="I11" t="s">
+        <v>246</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E24A130-A769-514F-88AC-721079C11998}">
+  <dimension ref="A1:J3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:J1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I2" t="s">
+        <v>93</v>
+      </c>
+      <c r="J2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G3" t="s">
         <v>99</v>
       </c>
-      <c r="C2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8625C5A4-1B9A-3246-B25B-1B4BBC206FFB}">
+  <dimension ref="A1:L10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="20.33203125" customWidth="1"/>
+    <col min="8" max="9" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>118</v>
+      </c>
+      <c r="G2" t="s">
+        <v>119</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="J2" t="s">
+        <v>121</v>
+      </c>
+      <c r="K2" t="s">
+        <v>122</v>
+      </c>
+      <c r="L2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>104</v>
-      </c>
-      <c r="B3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C3" t="s">
-        <v>98</v>
+        <v>123</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="D3" t="s">
-        <v>113</v>
-      </c>
-      <c r="E3" t="s">
-        <v>110</v>
-      </c>
-      <c r="F3" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="G3" t="s">
-        <v>115</v>
-      </c>
-      <c r="H3" t="s">
-        <v>116</v>
+        <v>176</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>126</v>
       </c>
       <c r="I3" t="s">
-        <v>111</v>
+        <v>127</v>
+      </c>
+      <c r="L3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="D4" t="s">
+        <v>131</v>
+      </c>
+      <c r="G4" t="s">
+        <v>176</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="I4" t="s">
+        <v>132</v>
+      </c>
+      <c r="K4" t="s">
+        <v>133</v>
+      </c>
+      <c r="L4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D5" t="s">
+        <v>137</v>
+      </c>
+      <c r="E5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F5" t="s">
+        <v>77</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I5" t="s">
+        <v>138</v>
+      </c>
+      <c r="K5" t="s">
+        <v>139</v>
+      </c>
+      <c r="L5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D6" t="s">
+        <v>143</v>
+      </c>
+      <c r="G6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="I6" t="s">
+        <v>144</v>
+      </c>
+      <c r="L6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>145</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
+        <v>147</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I7" t="s">
+        <v>44</v>
+      </c>
+      <c r="L7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>148</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D8" t="s">
+        <v>151</v>
+      </c>
+      <c r="G8" t="s">
+        <v>152</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="L8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>154</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="D9" t="s">
+        <v>157</v>
+      </c>
+      <c r="E9" t="s">
+        <v>77</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="I9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>161</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="D10" t="s">
+        <v>164</v>
+      </c>
+      <c r="G10" t="s">
+        <v>176</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="I10" t="s">
+        <v>165</v>
+      </c>
+      <c r="L10" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>